<commit_message>
Tested two testcases related to TeamLead Login and TeamLead
</commit_message>
<xml_diff>
--- a/TestCases/Back End/DeleteAssessment-BackEnd-TeamLead.xlsx
+++ b/TestCases/Back End/DeleteAssessment-BackEnd-TeamLead.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18801"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{9C129D2C-0248-475A-B2A1-8D8FB6DD6AB3}" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{629898E5-A087-4850-9F11-55A28D07BCA2}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{9C129D2C-0248-475A-B2A1-8D8FB6DD6AB3}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{00C083CE-8B68-4B08-AA57-49DC5E65576D}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
-    <t xml:space="preserve">Role: Team Lead </t>
+    <t>Role: Team Lead </t>
   </si>
   <si>
     <t>Test Case: Testing to see if deleting an assessment affects it in the database</t>
@@ -403,9 +403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>